<commit_message>
University import,export and bulk update via import
</commit_message>
<xml_diff>
--- a/public/format/university.xlsx
+++ b/public/format/university.xlsx
@@ -22,44 +22,44 @@
     <t>institute_type_id</t>
   </si>
   <si>
-    <t>country</t>
-  </si>
-  <si>
     <t>state</t>
   </si>
   <si>
     <t>city</t>
   </si>
   <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>founded</t>
-  </si>
-  <si>
-    <t>university_rank</t>
-  </si>
-  <si>
-    <t>destination_id</t>
-  </si>
-  <si>
     <t>qs_rank</t>
   </si>
   <si>
-    <t>us_world_rank</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>parent_university_id</t>
+    <t>shortnote</t>
+  </si>
+  <si>
+    <t>views</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>rank</t>
+  </si>
+  <si>
+    <t>times_rank</t>
+  </si>
+  <si>
+    <t>latitude_longitude</t>
+  </si>
+  <si>
+    <t>featured</t>
+  </si>
+  <si>
+    <t>established_year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +191,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -537,8 +544,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -894,43 +902,44 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>